<commit_message>
SVM+GL for Chinese character, CNN+GL for single digit
</commit_message>
<xml_diff>
--- a/digit_digit_matrix_64/Results/CNN_with_GL.xlsx
+++ b/digit_digit_matrix_64/Results/CNN_with_GL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\Group_Learning\digit_digit_matrix_64\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D62CBD-A45D-4518-97E5-8F98EC6F8D74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD5A95B-5E31-48EC-A85A-2B231F0F3EF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{97F154ED-AFD4-4F8B-AC9B-273AA66C97F5}"/>
   </bookViews>
@@ -16,10 +16,6 @@
     <sheet name="CNN" sheetId="1" r:id="rId1"/>
     <sheet name="CNN+GL_differ_window_size" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'CNN+GL_differ_window_size'!$B$21:$F$21</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">('CNN+GL_differ_window_size'!$B$8,'CNN+GL_differ_window_size'!$H$8,'CNN+GL_differ_window_size'!$N$8,'CNN+GL_differ_window_size'!$T$8,'CNN+GL_differ_window_size'!$Z$8)</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2605,6 +2601,1178 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>CNN+GL</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'CNN+GL_differ_window_size'!$B$23:$M$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('CNN+GL_differ_window_size'!$C$10,'CNN+GL_differ_window_size'!$I$10,'CNN+GL_differ_window_size'!$C$20,'CNN+GL_differ_window_size'!$I$20,'CNN+GL_differ_window_size'!$O$10,'CNN+GL_differ_window_size'!$O$20,'CNN+GL_differ_window_size'!$U$20,'CNN+GL_differ_window_size'!$AA$20,'CNN+GL_differ_window_size'!$AG$20,'CNN+GL_differ_window_size'!$AM$20,'CNN+GL_differ_window_size'!$U$10,'CNN+GL_differ_window_size'!$AA$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.000000000000008E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DEEE-4CAD-A997-7648DED7819C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="537757744"/>
+        <c:axId val="537761352"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>CNN</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'CNN+GL_differ_window_size'!$B$23:$M$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CNN!$G$12:$R$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-DEEE-4CAD-A997-7648DED7819C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="537757744"/>
+        <c:axId val="537761352"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="537757744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1400">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Window</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1400" baseline="0">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t> size</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1400">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="537761352"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="537761352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1400">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Training</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1400" baseline="0">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t> error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="537757744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>CNN+GL</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'CNN+GL_differ_window_size'!$B$23:$M$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('CNN+GL_differ_window_size'!$E$10,'CNN+GL_differ_window_size'!$K$10,'CNN+GL_differ_window_size'!$E$20,'CNN+GL_differ_window_size'!$K$20,'CNN+GL_differ_window_size'!$Q$10,'CNN+GL_differ_window_size'!$Q$20,'CNN+GL_differ_window_size'!$W$20,'CNN+GL_differ_window_size'!$AC$20,'CNN+GL_differ_window_size'!$AI$20,'CNN+GL_differ_window_size'!$AO$20,'CNN+GL_differ_window_size'!$W$10,'CNN+GL_differ_window_size'!$AC$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.49129999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28980000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.1799999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.3200000000000052E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.10519999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.10880000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.11019999999999985</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.11139999999999994</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.10299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.4000000000000048E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.0000000000000053E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1BDC-428E-9A66-F8F8F76D79CC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="537757744"/>
+        <c:axId val="537761352"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>CNN</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'CNN+GL_differ_window_size'!$B$23:$M$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CNN!$G$11:$R$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.79139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.79139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.79139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.79139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.79139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.79139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.79139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.79139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.79139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.79139999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1BDC-428E-9A66-F8F8F76D79CC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="537757744"/>
+        <c:axId val="537761352"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="537757744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1400">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Window</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1400" baseline="0">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t> size</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1400">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="537761352"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="537761352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1400">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Test</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-TW" sz="1400" baseline="0">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t> error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-TW"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="537757744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2765,6 +3933,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4810,6 +6058,1012 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4976,6 +7230,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>368850</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>144420</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="圖表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{788D0677-E2AB-4EAD-ADB0-4B2BABBC6272}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>433620</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>45360</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="圖表 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C48E442-A1F0-4181-B070-E05E93E8840F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5281,10 +7609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F1EE36-F344-4E97-B968-490B99892719}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -5293,12 +7621,12 @@
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -5315,7 +7643,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5332,7 +7660,7 @@
         <v>0.996</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>2</v>
       </c>
@@ -5349,7 +7677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>3</v>
       </c>
@@ -5366,7 +7694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>4</v>
       </c>
@@ -5383,7 +7711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>5</v>
       </c>
@@ -5400,7 +7728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:18">
       <c r="B8">
         <f>AVERAGE(B3:B7)</f>
         <v>1</v>
@@ -5416,6 +7744,93 @@
       <c r="E8">
         <f t="shared" si="0"/>
         <v>0.19919999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="C10">
+        <f>AVERAGE(B8:C8)</f>
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ref="E10" si="1">AVERAGE(D8:E8)</f>
+        <v>0.20860000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="G11">
+        <f>1-E10</f>
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="H11">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="I11">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="J11">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="K11">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="L11">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="M11">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="N11">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="O11">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="P11">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="Q11">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="R11">
+        <v>0.79139999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5429,8 +7844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74FD9C25-746F-40BA-B3EB-61B6AEA4F796}">
   <dimension ref="A1:AO23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView tabSelected="1" topLeftCell="L31" workbookViewId="0">
+      <selection activeCell="AC39" sqref="AC39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2"/>
@@ -6097,6 +8512,48 @@
         <v>4.2614551505325025E-2</v>
       </c>
     </row>
+    <row r="10" spans="1:41">
+      <c r="C10">
+        <f>1-AVERAGE(B8:C8)</f>
+        <v>0.36</v>
+      </c>
+      <c r="E10">
+        <f>1-AVERAGE(D8:E8)</f>
+        <v>0.49129999999999996</v>
+      </c>
+      <c r="I10">
+        <f>1-AVERAGE(H8:I8)</f>
+        <v>9.000000000000008E-2</v>
+      </c>
+      <c r="K10">
+        <f>1-AVERAGE(J8:K8)</f>
+        <v>0.28980000000000006</v>
+      </c>
+      <c r="O10">
+        <f>1-AVERAGE(N8:O8)</f>
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <f>1-AVERAGE(P8:Q8)</f>
+        <v>8.3200000000000052E-2</v>
+      </c>
+      <c r="U10">
+        <f>1-AVERAGE(T8:U8)</f>
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <f>1-AVERAGE(V8:W8)</f>
+        <v>5.4000000000000048E-2</v>
+      </c>
+      <c r="AA10">
+        <f>1-AVERAGE(Z8:AA8)</f>
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <f>1-AVERAGE(AB8:AC8)</f>
+        <v>6.0000000000000053E-2</v>
+      </c>
+    </row>
     <row r="11" spans="1:41">
       <c r="A11" t="s">
         <v>6</v>
@@ -6930,14 +9387,6 @@
         <f t="shared" si="8"/>
         <v>1.9975985582694054E-2</v>
       </c>
-      <c r="L19" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="8"/>
-        <v>1.4142135623730951</v>
-      </c>
       <c r="N19">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -7017,6 +9466,64 @@
       <c r="AO19">
         <f t="shared" si="8"/>
         <v>1.3564659966250548E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41">
+      <c r="C20">
+        <f>1-AVERAGE(B18:C18)</f>
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f>1-AVERAGE(D18:E18)</f>
+        <v>9.1799999999999993E-2</v>
+      </c>
+      <c r="I20">
+        <f>1-AVERAGE(H18:I18)</f>
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <f>1-AVERAGE(J18:K18)</f>
+        <v>0.1008</v>
+      </c>
+      <c r="O20">
+        <f>1-AVERAGE(N18:O18)</f>
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <f>1-AVERAGE(P18:Q18)</f>
+        <v>0.10519999999999996</v>
+      </c>
+      <c r="U20">
+        <f>1-AVERAGE(T18:U18)</f>
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <f>1-AVERAGE(V18:W18)</f>
+        <v>0.10880000000000001</v>
+      </c>
+      <c r="AA20">
+        <f>1-AVERAGE(Z18:AA18)</f>
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <f>1-AVERAGE(AB18:AC18)</f>
+        <v>0.11019999999999985</v>
+      </c>
+      <c r="AG20">
+        <f>1-AVERAGE(AF18:AG18)</f>
+        <v>0</v>
+      </c>
+      <c r="AI20">
+        <f>1-AVERAGE(AH18:AI18)</f>
+        <v>0.11139999999999994</v>
+      </c>
+      <c r="AM20">
+        <f>1-AVERAGE(AL18:AM18)</f>
+        <v>0</v>
+      </c>
+      <c r="AO20">
+        <f>1-AVERAGE(AN18:AO18)</f>
+        <v>0.10299999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:41">

</xml_diff>